<commit_message>
change all condition into assert
</commit_message>
<xml_diff>
--- a/Resources/TestData/Control_File2.xlsx
+++ b/Resources/TestData/Control_File2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19dcfb542a800ec3/سطح المكتب/Octopus-master/Resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{67A066BB-34FC-41C4-933D-69264051F4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA857025-C9C8-494E-A0EF-0188DD2BB4A1}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{67A066BB-34FC-41C4-933D-69264051F4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{967DB5C5-FB60-456F-BC45-D380F4653938}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" activeTab="1" xr2:uid="{7AC7F635-5FAF-4421-ACA9-E1DE0404826F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -274,10 +274,7 @@
     <t>Lion</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>no</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -601,6 +598,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1159,7 +1160,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1276,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>37</v>
@@ -1295,7 +1296,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>37</v>
@@ -1379,7 +1380,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="111" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>